<commit_message>
Version archivos 10 junio 2020
Versión archivos 10 junio 2020
</commit_message>
<xml_diff>
--- a/2020/cursos/etica/Noveno/Listados Etica 9-1.xlsx
+++ b/2020/cursos/etica/Noveno/Listados Etica 9-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\cursos\etica\Noveno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34487E10-03D0-43D2-A285-CF428075AA9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA9B4C-AFB8-40B3-8D58-42794738D4AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="3435" windowWidth="14400" windowHeight="10755" xr2:uid="{1EA2306F-59E9-4E0F-8411-BCE0FE820673}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14400" windowHeight="13710" xr2:uid="{1EA2306F-59E9-4E0F-8411-BCE0FE820673}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>Codigo</t>
   </si>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +175,13 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,6 +241,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD09D4E-2993-4F11-BB0F-40F78899A78D}">
   <dimension ref="A3:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +665,9 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
+      <c r="D9" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -719,6 +732,9 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
+      <c r="D14" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1013,6 +1029,9 @@
       </c>
       <c r="C37" t="s">
         <v>36</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -1023,7 +1042,7 @@
       </c>
       <c r="D38" s="8">
         <f>COUNTA(D4:D37)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>